<commit_message>
created test script vacancies
</commit_message>
<xml_diff>
--- a/test_data/test_data.xlsx
+++ b/test_data/test_data.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="empentitlements" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="vacancies" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>username</t>
   </si>
@@ -40,6 +40,30 @@
   </si>
   <si>
     <t>Peter Mac</t>
+  </si>
+  <si>
+    <t>Job Title</t>
+  </si>
+  <si>
+    <t>Vacancy</t>
+  </si>
+  <si>
+    <t>Hiring manager</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Tester TopGun</t>
+  </si>
+  <si>
+    <t>Tester01</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Anthony Nolan</t>
   </si>
 </sst>
 </file>
@@ -411,7 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -445,12 +469,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>